<commit_message>
Add OA_TEST.xlsx data file to the project
</commit_message>
<xml_diff>
--- a/quickshift/src/datafiles/MiMalla.xlsx
+++ b/quickshift/src/datafiles/MiMalla.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28740" windowHeight="11400" tabRatio="500"/>
+    <workbookView windowWidth="14400" windowHeight="12600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MiMalla" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="140">
   <si>
     <t>Mi Malla Curricular 
 (modificar el año de la
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t xml:space="preserve">Requisitos </t>
+  </si>
+  <si>
+    <t>Electivo</t>
   </si>
   <si>
     <t>Álgebra y Geometría</t>
@@ -443,10 +446,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -512,92 +515,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -612,6 +532,67 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -619,7 +600,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -628,6 +609,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -642,10 +630,25 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -730,7 +733,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -742,7 +757,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -754,7 +775,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,115 +877,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -967,7 +970,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -976,7 +979,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1018,150 +1021,150 @@
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1169,13 +1172,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="31" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="32" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1196,20 +1202,20 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="12" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1222,20 +1228,20 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="12" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Excel Built-in Calculation" xfId="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Excel Built-in Calculation" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -1781,14 +1787,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Malla_20" displayName="Malla_20" ref="A1:E57" totalsRowShown="0">
-  <autoFilter ref="A1:E57"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Malla_20" displayName="Malla_20" ref="A1:F57" totalsRowShown="0">
+  <autoFilter ref="A1:F57"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Nombre" dataDxfId="0"/>
     <tableColumn id="2" name="ID" dataDxfId="1"/>
     <tableColumn id="3" name="Créditos" dataDxfId="2"/>
     <tableColumn id="4" name="Requisitos " dataDxfId="3"/>
     <tableColumn id="5" name="Semestre" dataDxfId="4"/>
+    <tableColumn id="6" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2082,7 +2089,7 @@
   <sheetPr/>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2091,607 +2098,607 @@
     <col min="1" max="1" width="29.2833333333333" customWidth="1"/>
     <col min="2" max="2" width="26.425" customWidth="1"/>
     <col min="3" max="3" width="34.1416666666667" customWidth="1"/>
-    <col min="4" max="4" width="24.85" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.85" style="4" customWidth="1"/>
     <col min="5" max="5" width="18.425" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="47.25" customHeight="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-      <c r="E3" s="26" t="s">
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="8">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="26" t="s">
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="8">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="26" t="s">
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="26">
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="27">
         <v>9</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="8">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="12">
         <v>1</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="10">
+      <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="12">
         <v>2</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="10">
+      <c r="A10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="12">
         <v>2</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="10">
+      <c r="A11" s="11">
         <v>9</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="12">
         <v>4</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="10">
+      <c r="A12" s="11">
         <v>10</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="11">
-        <v>0</v>
-      </c>
-      <c r="E12" s="28" t="s">
+      <c r="D12" s="12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="12">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="31">
         <v>18</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="12">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="14">
         <v>7</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="12">
+      <c r="A15" s="13">
         <v>13</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="12">
+      <c r="A16" s="13">
         <v>14</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="14">
         <v>9</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="31">
         <v>19</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="12">
+      <c r="A17" s="13">
         <v>15</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="14">
         <v>9</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="14">
+      <c r="A18" s="15">
         <v>16</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="34">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="14">
+      <c r="A19" s="15">
         <v>17</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="34">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="14">
+      <c r="A20" s="15">
         <v>18</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="33">
         <v>23</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="34">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="14">
+      <c r="A21" s="15">
         <v>19</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="16">
         <v>14</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="34">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="14">
+      <c r="A22" s="15">
         <v>20</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="15">
-        <v>0</v>
-      </c>
-      <c r="E22" s="32" t="s">
+      <c r="D22" s="16">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="34">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
-      <c r="I25" s="44"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="36"/>
+      <c r="I25" s="45"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="35"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="36"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="37"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="40"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="39"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="40"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="40"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="41"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="42"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="41"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="42"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="41"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="42"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="43"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="44"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="43"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="44"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="43"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="44"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="43"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2704,15 +2711,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="29.25" spans="1:5">
+    <row r="1" ht="29.25" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -2728,10 +2738,13 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="43.5" spans="1:5">
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" ht="29.25" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -2740,15 +2753,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:5">
+      <c r="F2" s="3" t="b">
+        <f t="shared" ref="F2:F48" si="0">A2="Electivo Profesional"</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -2757,15 +2774,19 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" spans="1:5">
+      <c r="F3" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -2774,15 +2795,19 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" ht="29.25" spans="1:5">
+      <c r="F4" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -2791,15 +2816,19 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" ht="57.75" spans="1:5">
+      <c r="F5" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="29.25" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -2808,15 +2837,19 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" ht="29.25" spans="1:5">
+      <c r="F6" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -2830,10 +2863,14 @@
       <c r="E7" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" ht="15.75" spans="1:5">
+      <c r="F7" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -2847,10 +2884,14 @@
       <c r="E8" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" ht="15.75" spans="1:5">
+      <c r="F8" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -2864,10 +2905,14 @@
       <c r="E9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" ht="43.5" spans="1:5">
+      <c r="F9" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" ht="29.25" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -2881,10 +2926,14 @@
       <c r="E10" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" ht="43.5" spans="1:5">
+      <c r="F10" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" ht="29.25" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -2893,15 +2942,19 @@
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" ht="57.75" spans="1:5">
+      <c r="F11" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="29.25" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -2915,10 +2968,14 @@
       <c r="E12" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" ht="15.75" spans="1:5">
+      <c r="F12" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -2932,10 +2989,14 @@
       <c r="E13" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" ht="29.25" spans="1:5">
+      <c r="F13" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -2949,10 +3010,14 @@
       <c r="E14" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" ht="72" spans="1:5">
+      <c r="F14" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" ht="29.25" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -2966,10 +3031,14 @@
       <c r="E15" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" ht="29.25" spans="1:5">
+      <c r="F15" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -2983,10 +3052,14 @@
       <c r="E16" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" ht="57.75" spans="1:5">
+      <c r="F16" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" ht="29.25" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -3000,10 +3073,14 @@
       <c r="E17" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" ht="57.75" spans="1:5">
+      <c r="F17" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" ht="29.25" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -3017,10 +3094,14 @@
       <c r="E18" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" ht="57.75" spans="1:5">
+      <c r="F18" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" ht="29.25" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -3034,10 +3115,14 @@
       <c r="E19" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" ht="29.25" spans="1:5">
+      <c r="F19" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -3051,10 +3136,14 @@
       <c r="E20" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" ht="43.5" spans="1:5">
+      <c r="F20" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" ht="29.25" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
@@ -3068,10 +3157,14 @@
       <c r="E21" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" ht="15.75" spans="1:5">
+      <c r="F21" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B22" s="2">
         <v>21</v>
@@ -3080,15 +3173,19 @@
         <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" ht="29.25" spans="1:5">
+      <c r="F22" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B23" s="2">
         <v>22</v>
@@ -3102,10 +3199,14 @@
       <c r="E23" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" ht="43.5" spans="1:5">
+      <c r="F23" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" ht="29.25" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B24" s="2">
         <v>23</v>
@@ -3119,10 +3220,14 @@
       <c r="E24" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" ht="29.25" spans="1:5">
+      <c r="F24" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B25" s="2">
         <v>24</v>
@@ -3136,10 +3241,14 @@
       <c r="E25" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" ht="57.75" spans="1:5">
+      <c r="F25" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" ht="29.25" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B26" s="2">
         <v>25</v>
@@ -3153,10 +3262,14 @@
       <c r="E26" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" ht="43.5" spans="1:5">
+      <c r="F26" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" ht="29.25" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2">
         <v>26</v>
@@ -3165,15 +3278,19 @@
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E27" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" ht="15.75" spans="1:5">
+      <c r="F27" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B28" s="2">
         <v>27</v>
@@ -3187,10 +3304,14 @@
       <c r="E28" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" ht="43.5" spans="1:5">
+      <c r="F28" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" ht="29.25" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B29" s="2">
         <v>28</v>
@@ -3199,18 +3320,22 @@
         <v>6</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E29" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" ht="86.25" spans="1:5">
+      <c r="F29" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" ht="43.5" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B30" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2">
         <v>6</v>
@@ -3221,13 +3346,17 @@
       <c r="E30" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" ht="29.25" spans="1:5">
+      <c r="F30" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" ht="29.25" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B31" s="2">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31" s="2">
         <v>6</v>
@@ -3238,10 +3367,14 @@
       <c r="E31" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" ht="43.5" spans="1:5">
+      <c r="F31" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" ht="29.25" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B32" s="2">
         <v>31</v>
@@ -3255,10 +3388,14 @@
       <c r="E32" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" ht="43.5" spans="1:5">
+      <c r="F32" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" ht="29.25" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2">
         <v>32</v>
@@ -3267,15 +3404,19 @@
         <v>5</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E33" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" ht="15.75" spans="1:5">
+      <c r="F33" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2">
         <v>33</v>
@@ -3289,10 +3430,14 @@
       <c r="E34" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" ht="43.5" spans="1:5">
+      <c r="F34" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" ht="29.25" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B35" s="2">
         <v>34</v>
@@ -3306,10 +3451,14 @@
       <c r="E35" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" ht="43.5" spans="1:5">
+      <c r="F35" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" ht="29.25" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B36" s="2">
         <v>35</v>
@@ -3323,10 +3472,14 @@
       <c r="E36" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" ht="43.5" spans="1:5">
+      <c r="F36" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" ht="29.25" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B37" s="2">
         <v>36</v>
@@ -3340,10 +3493,14 @@
       <c r="E37" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" ht="43.5" spans="1:5">
+      <c r="F37" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" ht="29.25" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B38" s="2">
         <v>37</v>
@@ -3357,10 +3514,14 @@
       <c r="E38" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" ht="43.5" spans="1:5">
+      <c r="F38" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" ht="29.25" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" s="2">
         <v>38</v>
@@ -3369,15 +3530,19 @@
         <v>5</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E39" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" ht="43.5" spans="1:5">
+      <c r="F39" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" ht="29.25" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B40" s="2">
         <v>39</v>
@@ -3386,15 +3551,19 @@
         <v>7</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E40" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" ht="57.75" spans="1:5">
+      <c r="F40" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" ht="29.25" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B41" s="2">
         <v>40</v>
@@ -3408,10 +3577,14 @@
       <c r="E41" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" ht="57.75" spans="1:5">
+      <c r="F41" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" ht="43.5" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B42" s="2">
         <v>41</v>
@@ -3425,10 +3598,14 @@
       <c r="E42" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" ht="29.25" spans="1:5">
+      <c r="F42" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B43" s="2">
         <v>42</v>
@@ -3437,15 +3614,19 @@
         <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E43" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" ht="57.75" spans="1:5">
+      <c r="F43" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" ht="29.25" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B44" s="2">
         <v>43</v>
@@ -3454,15 +3635,19 @@
         <v>6</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E44" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" ht="43.5" spans="1:5">
+      <c r="F44" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" ht="29.25" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B45" s="2">
         <v>55</v>
@@ -3476,10 +3661,14 @@
       <c r="E45" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" ht="43.5" spans="1:5">
+      <c r="F45" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" ht="29.25" spans="1:6">
       <c r="A46" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46" s="2">
         <v>44</v>
@@ -3488,15 +3677,19 @@
         <v>6</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E46" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" ht="57.75" spans="1:5">
+      <c r="F46" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" ht="29.25" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B47" s="2">
         <v>45</v>
@@ -3510,10 +3703,14 @@
       <c r="E47" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" ht="43.5" spans="1:5">
+      <c r="F47" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" ht="29.25" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B48" s="2">
         <v>46</v>
@@ -3522,15 +3719,19 @@
         <v>6</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E48" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" ht="43.5" spans="1:5">
+      <c r="F48" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" ht="29.25" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B49" s="2">
         <v>50</v>
@@ -3539,15 +3740,19 @@
         <v>6</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E49" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" ht="43.5" spans="1:5">
+      <c r="F49" s="3" t="b">
+        <f t="shared" ref="F49:F57" si="1">A49="Electivo Profesional"</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" ht="29.25" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B50" s="2">
         <v>47</v>
@@ -3561,10 +3766,14 @@
       <c r="E50" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" ht="29.25" spans="1:5">
+      <c r="F50" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B51" s="2">
         <v>48</v>
@@ -3578,10 +3787,14 @@
       <c r="E51" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" ht="29.25" spans="1:5">
+      <c r="F51" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B52" s="2">
         <v>53</v>
@@ -3595,10 +3808,14 @@
       <c r="E52" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" ht="43.5" spans="1:5">
+      <c r="F52" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" ht="29.25" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B53" s="2">
         <v>51</v>
@@ -3607,15 +3824,19 @@
         <v>6</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E53" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="54" ht="43.5" spans="1:5">
+      <c r="F53" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" ht="29.25" spans="1:6">
       <c r="A54" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B54" s="2">
         <v>52</v>
@@ -3624,49 +3845,61 @@
         <v>6</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E54" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" ht="43.5" spans="1:5">
+      <c r="F54" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" ht="29.25" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B55" s="2">
         <v>56</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E55" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" ht="114.75" spans="1:5">
+      <c r="F55" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" ht="72" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E56" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="57" ht="43.5" spans="1:5">
+      <c r="F56" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" ht="29.25" spans="1:6">
       <c r="A57" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B57" s="2">
         <v>54</v>
@@ -3675,10 +3908,14 @@
         <v>7</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="F57" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3721,9 +3958,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="43.5" spans="1:5">
+    <row r="2" ht="15.75" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -3732,7 +3969,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -3740,7 +3977,7 @@
     </row>
     <row r="3" ht="15.75" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -3749,7 +3986,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -3757,7 +3994,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -3766,15 +4003,15 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="29.25" spans="1:5">
+    <row r="5" ht="15.75" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -3783,15 +4020,15 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="57.75" spans="1:5">
+    <row r="6" ht="15.75" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -3800,15 +4037,15 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" ht="29.25" spans="1:5">
+    <row r="7" ht="15.75" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -3825,7 +4062,7 @@
     </row>
     <row r="8" ht="15.75" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -3842,7 +4079,7 @@
     </row>
     <row r="9" ht="15.75" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -3857,9 +4094,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" ht="43.5" spans="1:5">
+    <row r="10" ht="15.75" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -3874,26 +4111,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" ht="29.25" spans="1:5">
+    <row r="11" ht="15.75" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" ht="57.75" spans="1:5">
+    <row r="12" ht="15.75" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -3910,7 +4147,7 @@
     </row>
     <row r="13" ht="15.75" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -3925,9 +4162,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" ht="29.25" spans="1:5">
+    <row r="14" ht="15.75" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -3942,9 +4179,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" ht="43.5" spans="1:5">
+    <row r="15" ht="15.75" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -3959,9 +4196,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" ht="29.25" spans="1:5">
+    <row r="16" ht="15.75" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -3976,9 +4213,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" ht="57.75" spans="1:5">
+    <row r="17" ht="15.75" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -3993,9 +4230,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" ht="43.5" spans="1:5">
+    <row r="18" ht="15.75" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -4010,9 +4247,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" ht="57.75" spans="1:5">
+    <row r="19" ht="15.75" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -4027,9 +4264,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" ht="72" spans="1:5">
+    <row r="20" ht="15.75" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -4044,18 +4281,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" ht="29.25" spans="1:5">
+    <row r="21" ht="15.75" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" s="2">
         <v>4</v>
@@ -4063,7 +4300,7 @@
     </row>
     <row r="22" ht="15.75" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B22" s="2">
         <v>21</v>
@@ -4072,15 +4309,15 @@
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="23" ht="29.25" spans="1:5">
+    <row r="23" ht="15.75" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B23" s="2">
         <v>22</v>
@@ -4089,15 +4326,15 @@
         <v>6</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="24" ht="57.75" spans="1:5">
+    <row r="24" ht="15.75" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B24" s="2">
         <v>23</v>
@@ -4112,9 +4349,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" ht="29.25" spans="1:5">
+    <row r="25" ht="15.75" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B25" s="2">
         <v>24</v>
@@ -4123,15 +4360,15 @@
         <v>6</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E25" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="26" ht="29.25" spans="1:5">
+    <row r="26" ht="15.75" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B26" s="2">
         <v>25</v>
@@ -4146,18 +4383,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" ht="29.25" spans="1:5">
+    <row r="27" ht="15.75" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B27" s="2">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E27" s="2">
         <v>5</v>
@@ -4165,7 +4402,7 @@
     </row>
     <row r="28" ht="15.75" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B28" s="2">
         <v>27</v>
@@ -4180,9 +4417,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" ht="43.5" spans="1:5">
+    <row r="29" ht="15.75" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B29" s="2">
         <v>28</v>
@@ -4191,15 +4428,15 @@
         <v>6</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E29" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="30" ht="43.5" spans="1:5">
+    <row r="30" ht="15.75" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B30" s="2">
         <v>29</v>
@@ -4208,15 +4445,15 @@
         <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E30" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="31" ht="29.25" spans="1:5">
+    <row r="31" ht="15.75" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B31" s="2">
         <v>30</v>
@@ -4225,15 +4462,15 @@
         <v>6</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E31" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="32" ht="43.5" spans="1:5">
+    <row r="32" ht="15.75" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B32" s="2">
         <v>31</v>
@@ -4242,15 +4479,15 @@
         <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E32" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="33" ht="29.25" spans="1:5">
+    <row r="33" ht="15.75" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B33" s="2">
         <v>32</v>
@@ -4267,7 +4504,7 @@
     </row>
     <row r="34" ht="15.75" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2">
         <v>33</v>
@@ -4282,9 +4519,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" ht="43.5" spans="1:5">
+    <row r="35" ht="15.75" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B35" s="2">
         <v>34</v>
@@ -4293,15 +4530,15 @@
         <v>5</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E35" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="36" ht="43.5" spans="1:5">
+    <row r="36" ht="15.75" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2">
         <v>35</v>
@@ -4316,9 +4553,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" ht="43.5" spans="1:5">
+    <row r="37" ht="15.75" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B37" s="2">
         <v>36</v>
@@ -4333,9 +4570,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" ht="43.5" spans="1:5">
+    <row r="38" ht="15.75" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B38" s="2">
         <v>37</v>
@@ -4344,15 +4581,15 @@
         <v>5</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E38" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="39" ht="57.75" spans="1:5">
+    <row r="39" ht="15.75" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B39" s="2">
         <v>38</v>
@@ -4367,9 +4604,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" ht="43.5" spans="1:5">
+    <row r="40" ht="15.75" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B40" s="2">
         <v>39</v>
@@ -4384,9 +4621,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" ht="43.5" spans="1:5">
+    <row r="41" ht="15.75" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B41" s="2">
         <v>40</v>
@@ -4395,15 +4632,15 @@
         <v>6</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E41" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="42" ht="57.75" spans="1:5">
+    <row r="42" ht="15.75" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B42" s="2">
         <v>41</v>
@@ -4412,15 +4649,15 @@
         <v>6</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E42" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="43" ht="57.75" spans="1:5">
+    <row r="43" ht="15.75" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B43" s="2">
         <v>42</v>
@@ -4435,26 +4672,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" ht="43.5" spans="1:5">
+    <row r="44" ht="15.75" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B44" s="2">
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E44" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="45" ht="57.75" spans="1:5">
+    <row r="45" ht="15.75" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B45" s="2">
         <v>44</v>
@@ -4469,43 +4706,43 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" ht="43.5" spans="1:5">
+    <row r="46" ht="15.75" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46" s="2">
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E46" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="47" ht="43.5" spans="1:5">
+    <row r="47" ht="15.75" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B47" s="2">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E47" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="48" ht="29.25" spans="1:5">
+    <row r="48" ht="15.75" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B48" s="2">
         <v>47</v>
@@ -4520,43 +4757,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" ht="43.5" spans="1:5">
+    <row r="49" ht="15.75" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B49" s="2">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E49" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="50" ht="43.5" spans="1:5">
+    <row r="50" ht="15.75" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B50" s="2">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E50" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="51" ht="43.5" spans="1:5">
+    <row r="51" ht="15.75" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B51" s="2">
         <v>50</v>
@@ -4571,18 +4808,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" ht="43.5" spans="1:5">
+    <row r="52" ht="15.75" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="2">
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E52" s="2">
         <v>11</v>
@@ -4627,7 +4864,7 @@
     </row>
     <row r="2" ht="43.5" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -4636,7 +4873,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -4644,7 +4881,7 @@
     </row>
     <row r="3" ht="15.75" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -4653,7 +4890,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -4661,7 +4898,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -4670,7 +4907,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -4678,7 +4915,7 @@
     </row>
     <row r="5" ht="29.25" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -4687,7 +4924,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -4695,7 +4932,7 @@
     </row>
     <row r="6" ht="57.75" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -4704,7 +4941,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -4712,7 +4949,7 @@
     </row>
     <row r="7" ht="29.25" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -4729,7 +4966,7 @@
     </row>
     <row r="8" ht="15.75" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -4746,7 +4983,7 @@
     </row>
     <row r="9" ht="15.75" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -4763,7 +5000,7 @@
     </row>
     <row r="10" ht="43.5" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -4780,16 +5017,16 @@
     </row>
     <row r="11" ht="29.25" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -4797,7 +5034,7 @@
     </row>
     <row r="12" ht="57.75" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -4814,7 +5051,7 @@
     </row>
     <row r="13" ht="15.75" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -4831,7 +5068,7 @@
     </row>
     <row r="14" ht="29.25" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -4848,7 +5085,7 @@
     </row>
     <row r="15" ht="43.5" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -4865,7 +5102,7 @@
     </row>
     <row r="16" ht="29.25" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -4882,7 +5119,7 @@
     </row>
     <row r="17" ht="57.75" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -4899,7 +5136,7 @@
     </row>
     <row r="18" ht="43.5" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -4916,7 +5153,7 @@
     </row>
     <row r="19" ht="57.75" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -4933,7 +5170,7 @@
     </row>
     <row r="20" ht="72" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -4950,16 +5187,16 @@
     </row>
     <row r="21" ht="29.25" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" s="2">
         <v>4</v>
@@ -4967,7 +5204,7 @@
     </row>
     <row r="22" ht="15.75" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B22" s="2">
         <v>21</v>
@@ -4976,7 +5213,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="2">
         <v>4</v>
@@ -4984,7 +5221,7 @@
     </row>
     <row r="23" ht="29.25" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B23" s="2">
         <v>22</v>
@@ -4993,7 +5230,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" s="2">
         <v>5</v>
@@ -5001,7 +5238,7 @@
     </row>
     <row r="24" ht="57.75" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B24" s="2">
         <v>23</v>
@@ -5018,13 +5255,13 @@
     </row>
     <row r="25" ht="29.25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B25" s="2">
         <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D25" s="2">
         <v>5</v>
@@ -5033,7 +5270,7 @@
     </row>
     <row r="26" ht="29.25" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B26" s="2">
         <v>25</v>
@@ -5050,16 +5287,16 @@
     </row>
     <row r="27" ht="29.25" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B27" s="2">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E27" s="2">
         <v>5</v>
@@ -5067,7 +5304,7 @@
     </row>
     <row r="28" ht="15.75" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B28" s="2">
         <v>27</v>
@@ -5084,7 +5321,7 @@
     </row>
     <row r="29" ht="43.5" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B29" s="2">
         <v>28</v>
@@ -5093,7 +5330,7 @@
         <v>6</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E29" s="2">
         <v>6</v>
@@ -5101,7 +5338,7 @@
     </row>
     <row r="30" ht="43.5" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B30" s="2">
         <v>29</v>
@@ -5110,7 +5347,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E30" s="2">
         <v>6</v>
@@ -5118,7 +5355,7 @@
     </row>
     <row r="31" ht="29.25" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B31" s="2">
         <v>30</v>
@@ -5127,7 +5364,7 @@
         <v>6</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E31" s="2">
         <v>6</v>
@@ -5135,7 +5372,7 @@
     </row>
     <row r="32" ht="43.5" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B32" s="2">
         <v>31</v>
@@ -5144,7 +5381,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E32" s="2">
         <v>6</v>
@@ -5152,7 +5389,7 @@
     </row>
     <row r="33" ht="29.25" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B33" s="2">
         <v>32</v>
@@ -5169,7 +5406,7 @@
     </row>
     <row r="34" ht="15.75" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2">
         <v>33</v>
@@ -5186,7 +5423,7 @@
     </row>
     <row r="35" ht="43.5" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B35" s="2">
         <v>34</v>
@@ -5203,7 +5440,7 @@
     </row>
     <row r="36" ht="43.5" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B36" s="2">
         <v>35</v>
@@ -5220,7 +5457,7 @@
     </row>
     <row r="37" ht="43.5" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B37" s="2">
         <v>36</v>
@@ -5229,7 +5466,7 @@
         <v>5</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E37" s="2">
         <v>7</v>
@@ -5237,7 +5474,7 @@
     </row>
     <row r="38" ht="57.75" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B38" s="2">
         <v>5</v>
@@ -5252,7 +5489,7 @@
     </row>
     <row r="39" ht="43.5" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B39" s="2">
         <v>38</v>
@@ -5269,7 +5506,7 @@
     </row>
     <row r="40" ht="43.5" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B40" s="2">
         <v>39</v>
@@ -5278,7 +5515,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E40" s="2">
         <v>8</v>
@@ -5286,7 +5523,7 @@
     </row>
     <row r="41" ht="57.75" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B41" s="2">
         <v>40</v>
@@ -5295,7 +5532,7 @@
         <v>6</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E41" s="2">
         <v>8</v>
@@ -5303,7 +5540,7 @@
     </row>
     <row r="42" ht="29.25" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B42" s="2">
         <v>41</v>
@@ -5312,7 +5549,7 @@
         <v>6</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E42" s="2">
         <v>8</v>
@@ -5320,7 +5557,7 @@
     </row>
     <row r="43" ht="57.75" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B43" s="2">
         <v>42</v>
@@ -5329,7 +5566,7 @@
         <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E43" s="2">
         <v>8</v>
@@ -5337,16 +5574,16 @@
     </row>
     <row r="44" ht="29.25" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B44" s="2">
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E44" s="2">
         <v>8</v>
@@ -5354,7 +5591,7 @@
     </row>
     <row r="45" ht="43.5" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B45" s="2">
         <v>44</v>
@@ -5363,7 +5600,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E45" s="2">
         <v>9</v>
@@ -5371,16 +5608,16 @@
     </row>
     <row r="46" ht="43.5" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46" s="2">
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E46" s="2">
         <v>9</v>
@@ -5388,16 +5625,16 @@
     </row>
     <row r="47" ht="43.5" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B47" s="2">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E47" s="2">
         <v>9</v>
@@ -5405,7 +5642,7 @@
     </row>
     <row r="48" ht="43.5" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B48" s="2">
         <v>47</v>
@@ -5414,7 +5651,7 @@
         <v>6</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E48" s="2">
         <v>10</v>
@@ -5422,16 +5659,16 @@
     </row>
     <row r="49" ht="43.5" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B49" s="2">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E49" s="2">
         <v>10</v>
@@ -5439,7 +5676,7 @@
     </row>
     <row r="50" ht="43.5" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B50" s="2">
         <v>49</v>
@@ -5448,7 +5685,7 @@
         <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E50" s="2">
         <v>10</v>
@@ -5456,16 +5693,16 @@
     </row>
     <row r="51" ht="43.5" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B51" s="2">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E51" s="2">
         <v>10</v>
@@ -5473,7 +5710,7 @@
     </row>
     <row r="52" ht="43.5" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B52" s="2">
         <v>51</v>
@@ -5490,7 +5727,7 @@
     </row>
     <row r="53" ht="43.5" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B53" s="2">
         <v>52</v>
@@ -5499,7 +5736,7 @@
         <v>6</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E53" s="2">
         <v>11</v>
@@ -5507,16 +5744,16 @@
     </row>
     <row r="54" ht="43.5" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B54" s="2">
         <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E54" s="2">
         <v>11</v>

</xml_diff>

<commit_message>
Initialize serverless project with Rust and Worker framework
- Add .gitignore to exclude target, node_modules, and .wrangler directories
- Create Cargo.toml for project configuration and dependencies
- Implement basic fetch event handler in lib.rs
- Configure wrangler.toml for project build settings
</commit_message>
<xml_diff>
--- a/quickshift/src/datafiles/MiMalla.xlsx
+++ b/quickshift/src/datafiles/MiMalla.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12600" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="13005" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MiMalla" sheetId="1" r:id="rId1"/>
@@ -446,10 +446,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -515,14 +515,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -538,8 +530,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -552,9 +584,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -562,6 +601,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -577,76 +646,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -745,7 +745,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -757,43 +781,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -805,25 +805,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,19 +829,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -865,19 +841,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -970,7 +970,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -979,7 +979,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,108 +1018,93 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
@@ -1112,55 +1112,55 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1180,8 +1180,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="32" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1202,20 +1202,20 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="12" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1228,20 +1228,20 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="12" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Excel Built-in Calculation" xfId="2"/>
+    <cellStyle name="Excel Built-in Calculation" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -2714,12 +2714,13 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B1" sqref="A1:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="29.25" spans="1:6">

</xml_diff>